<commit_message>
2019-09-17 16:36 repite test de aleatoriedad filtrando dificultades y agrega N a test pre tratamiento
</commit_message>
<xml_diff>
--- a/resultados/aleatoriedad-inicio/aleatoriedad-elo-reg.xlsx
+++ b/resultados/aleatoriedad-inicio/aleatoriedad-elo-reg.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="173">
   <si>
     <t>Indicador</t>
   </si>
@@ -74,217 +74,214 @@
     <t>Frac. Fácil ELO p7 c5</t>
   </si>
   <si>
-    <t>0.282 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.03 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.031 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.005 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.326 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.009 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.035 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.0 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.58 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.126 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.218 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.05 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.028 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.161 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.064 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.065 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.094 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.342 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.092 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.072 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.049 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.061 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.012 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.028 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.089 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.111 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.113 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.326 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.559 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.87 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.671 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.855 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.594 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.708 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.745 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.135 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.22 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.318 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.864 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.576 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.519 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.728 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.758 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.496 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.582 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.346 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.669 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.902 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.953 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.866 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.524 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.351 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.374 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.458 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.325 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.235 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.195 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.409 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.517 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.009 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.025 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.019 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.01 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.07 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.027 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.041 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.001 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.191 (N = 772)</t>
-  </si>
-  <si>
-    <t>0.051 (N = 772)</t>
-  </si>
-  <si>
-    <t>0.016 (N = 772)</t>
-  </si>
-  <si>
-    <t>0.013 (N = 772)</t>
+    <t>0.072 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.005 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.019 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.001 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.092 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.001 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.011 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.0 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.381 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.042 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.139 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.019 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.04 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.328 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.088 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.134 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.166 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.619 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.24 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.228 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.057 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.086 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.018 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.035 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.076 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.12 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.103 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.419 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.72 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.923 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.682 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.629 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.631 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.698 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.509 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.175 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.448 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.597 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.955 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.828 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.955 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.994 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.986 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.614 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.922 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.754 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.756 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.371 (N = 253)</t>
+  </si>
+  <si>
+    <t>0.494 (N = 253)</t>
+  </si>
+  <si>
+    <t>0.506 (N = 253)</t>
+  </si>
+  <si>
+    <t>0.105 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.077 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.101 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.296 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.155 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.038 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.07 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.288 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.002 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.015 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.026 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.018 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.075 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.058 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.121 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.014 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.131 (N = 1172)</t>
+  </si>
+  <si>
+    <t>0.064 (N = 1172)</t>
+  </si>
+  <si>
+    <t>0.025 (N = 1172)</t>
+  </si>
+  <si>
+    <t>0.006 (N = 1172)</t>
   </si>
   <si>
     <t>Frac. Difícil ELO p4 c3</t>
@@ -323,220 +320,220 @@
     <t>Frac. Difícil ELO p7 c5</t>
   </si>
   <si>
-    <t>0.998 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.933 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.806 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.724 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.757 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.192 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.408 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.186 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.403 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.072 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.379 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.161 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.207 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.03 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.252 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.143 (N = 210)</t>
-  </si>
-  <si>
-    <t>0.023 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.013 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.068 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.044 (N = 180)</t>
-  </si>
-  <si>
-    <t>0.004 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.025 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.12 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.054 (N = 150)</t>
-  </si>
-  <si>
-    <t>0.472 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.596 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.379 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.502 (N = 140)</t>
-  </si>
-  <si>
-    <t>0.015 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.162 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.082 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.32 (N = 120)</t>
-  </si>
-  <si>
-    <t>0.289 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.596 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.463 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.291 (N = 100)</t>
-  </si>
-  <si>
-    <t>0.926 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.933 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.74 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.572 (N = 354)</t>
-  </si>
-  <si>
-    <t>0.991 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.939 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.715 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.855 (N = 304)</t>
-  </si>
-  <si>
-    <t>0.633 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.755 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.609 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.686 (N = 254)</t>
-  </si>
-  <si>
-    <t>0.159 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.044 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.34 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.564 (N = 208)</t>
-  </si>
-  <si>
-    <t>0.215 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.091 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.419 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.697 (N = 178)</t>
-  </si>
-  <si>
-    <t>0.166 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.103 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.074 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.053 (N = 148)</t>
-  </si>
-  <si>
-    <t>0.834 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.356 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.537 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.445 (N = 1092)</t>
-  </si>
-  <si>
-    <t>0.352 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.073 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.182 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.325 (N = 932)</t>
-  </si>
-  <si>
-    <t>0.071 (N = 772)</t>
-  </si>
-  <si>
-    <t>0.088 (N = 772)</t>
-  </si>
-  <si>
-    <t>0.206 (N = 772)</t>
-  </si>
-  <si>
-    <t>0.073 (N = 772)</t>
+    <t>0.951 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.58 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.628 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.773 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.536 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.122 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.104 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.171 (N = 210)</t>
+  </si>
+  <si>
+    <t>0.45 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.218 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.519 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.59 (N = 195)</t>
+  </si>
+  <si>
+    <t>0.082 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.036 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.041 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.023 (N = 255)</t>
+  </si>
+  <si>
+    <t>0.043 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.056 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.013 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.024 (N = 240)</t>
+  </si>
+  <si>
+    <t>0.032 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.149 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.061 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.037 (N = 225)</t>
+  </si>
+  <si>
+    <t>0.366 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.439 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.152 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.177 (N = 170)</t>
+  </si>
+  <si>
+    <t>0.1 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.137 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.134 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.446 (N = 160)</t>
+  </si>
+  <si>
+    <t>0.505 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.42 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.308 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.372 (N = 150)</t>
+  </si>
+  <si>
+    <t>0.953 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.405 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.136 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.161 (N = 429)</t>
+  </si>
+  <si>
+    <t>0.948 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.43 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.202 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.253 (N = 404)</t>
+  </si>
+  <si>
+    <t>0.717 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.425 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.323 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.356 (N = 379)</t>
+  </si>
+  <si>
+    <t>0.445 (N = 253)</t>
+  </si>
+  <si>
+    <t>0.068 (N = 253)</t>
+  </si>
+  <si>
+    <t>0.353 (N = 253)</t>
+  </si>
+  <si>
+    <t>0.424 (N = 253)</t>
+  </si>
+  <si>
+    <t>0.732 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.153 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.649 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.776 (N = 238)</t>
+  </si>
+  <si>
+    <t>0.761 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.394 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.324 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.289 (N = 223)</t>
+  </si>
+  <si>
+    <t>0.792 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.072 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.044 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.071 (N = 1332)</t>
+  </si>
+  <si>
+    <t>0.603 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.033 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.027 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.112 (N = 1252)</t>
+  </si>
+  <si>
+    <t>0.537 (N = 1172)</t>
+  </si>
+  <si>
+    <t>0.229 (N = 1172)</t>
+  </si>
+  <si>
+    <t>0.145 (N = 1172)</t>
+  </si>
+  <si>
+    <t>0.132 (N = 1172)</t>
   </si>
 </sst>
 </file>
@@ -943,7 +940,7 @@
         <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -966,7 +963,7 @@
         <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -989,7 +986,7 @@
         <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1009,10 +1006,10 @@
         <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1032,10 +1029,10 @@
         <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1055,10 +1052,10 @@
         <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1078,10 +1075,10 @@
         <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1101,10 +1098,10 @@
         <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1124,10 +1121,10 @@
         <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1147,10 +1144,10 @@
         <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1161,7 +1158,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
         <v>52</v>
@@ -1170,10 +1167,10 @@
         <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1184,7 +1181,7 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
@@ -1193,10 +1190,10 @@
         <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1237,278 +1234,278 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>